<commit_message>
parcels xlsx update; mg icons
</commit_message>
<xml_diff>
--- a/data/District5_Parcels.xlsx
+++ b/data/District5_Parcels.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Projects\bitmaps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_Projects\bitmaps\git\District5\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C05861C-9F5D-453D-B261-E89EE7F68B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84D396A-C35B-4084-A411-45DFA298B589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="1605" windowWidth="22470" windowHeight="13845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="19">
   <si>
     <t>Tapped</t>
   </si>
@@ -47,12 +59,48 @@
   <si>
     <t>@_A_No1_</t>
   </si>
+  <si>
+    <t>bc1pdfvcfrep4tqp6uwz5z8w56060yzvgmsd4cdg3pu5g7j5g8g8axdqktvttc</t>
+  </si>
+  <si>
+    <t>@BitMap_News</t>
+  </si>
+  <si>
+    <t>@redfinalboss</t>
+  </si>
+  <si>
+    <t>bc1py2djl55dul739lc7kh5hse7zya7c6ennxg6dnhyhws8k6fl2uedsrm3l60</t>
+  </si>
+  <si>
+    <t>@TAKABITMAP</t>
+  </si>
+  <si>
+    <t>bc1pkqmljesfm3tpyq6ch3mdmy4x4faqjdkedzkgmup6ehjpvgsmdkssha3yf3</t>
+  </si>
+  <si>
+    <t>@OrionHyperloop</t>
+  </si>
+  <si>
+    <t>bc1pmxavyuug4qkmvuj6y053jlcjwvehf5q63lufcdpgrpc6mgqzf30qglj5mx</t>
+  </si>
+  <si>
+    <t>Reserved</t>
+  </si>
+  <si>
+    <t>@smol2247</t>
+  </si>
+  <si>
+    <t>@Dudeamoto</t>
+  </si>
+  <si>
+    <t>bc1pdkvsx7…</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +119,19 @@
     <font>
       <sz val="11"/>
       <color rgb="FF536471"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0F1419"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -101,13 +162,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,20 +455,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G2356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1515" workbookViewId="0">
-      <selection activeCell="G1533" sqref="G1533"/>
+    <sheetView tabSelected="1" topLeftCell="A1615" workbookViewId="0">
+      <selection activeCell="F1533" sqref="F1533"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" customWidth="1"/>
-    <col min="6" max="6" width="68.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="72.140625" style="6" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -414,7 +479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -425,7 +490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -436,7 +501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -447,7 +512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -458,7 +523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -469,7 +534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -479,8 +544,17 @@
       <c r="C7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -490,8 +564,17 @@
       <c r="C8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -501,8 +584,14 @@
       <c r="C9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -512,8 +601,17 @@
       <c r="C10" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -524,7 +622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -535,22 +633,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -8196,7 +8294,7 @@
         <v>1527</v>
       </c>
     </row>
-    <row r="1529" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="1529" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1529" s="1">
         <v>1528</v>
       </c>
@@ -8209,15 +8307,15 @@
       <c r="D1529" t="s">
         <v>2</v>
       </c>
-      <c r="E1529" s="2" t="s">
+      <c r="E1529" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1529" s="3" t="s">
+      <c r="F1529" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1529" s="4"/>
-    </row>
-    <row r="1530" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G1529" s="2"/>
+    </row>
+    <row r="1530" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1530" s="1">
         <v>1529</v>
       </c>
@@ -8230,15 +8328,15 @@
       <c r="D1530" t="s">
         <v>2</v>
       </c>
-      <c r="E1530" s="2" t="s">
+      <c r="E1530" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1530" s="3" t="s">
+      <c r="F1530" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1530" s="4"/>
-    </row>
-    <row r="1531" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="G1530" s="2"/>
+    </row>
+    <row r="1531" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1531" s="1">
         <v>1530</v>
       </c>
@@ -8251,15 +8349,15 @@
       <c r="D1531" t="s">
         <v>2</v>
       </c>
-      <c r="E1531" s="2" t="s">
+      <c r="E1531" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1531" s="3" t="s">
+      <c r="F1531" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1531" s="4"/>
-    </row>
-    <row r="1532" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G1531" s="2"/>
+    </row>
+    <row r="1532" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1532" s="1">
         <v>1531</v>
       </c>
@@ -8269,8 +8367,17 @@
       <c r="C1532" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="1533" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D1532" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1532" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1532" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1533" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1533" s="1">
         <v>1532</v>
       </c>
@@ -8280,8 +8387,17 @@
       <c r="C1533" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="1534" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="D1533" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1533" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1533" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="1534" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A1534" s="1">
         <v>1533</v>
       </c>
@@ -8294,10 +8410,10 @@
       <c r="D1534" t="s">
         <v>2</v>
       </c>
-      <c r="E1534" s="2" t="s">
+      <c r="E1534" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F1534" s="3" t="s">
+      <c r="F1534" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -8311,6 +8427,15 @@
       <c r="C1535" t="s">
         <v>0</v>
       </c>
+      <c r="D1535" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1535" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1535" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="1536" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1536" s="1">
@@ -8322,8 +8447,17 @@
       <c r="C1536" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="1537" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1536" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1536" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1536" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="1537" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1537" s="1">
         <v>1536</v>
       </c>
@@ -8333,78 +8467,87 @@
       <c r="C1537" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="1538" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1537" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1537" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1537" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1538" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1538" s="1">
         <v>1537</v>
       </c>
     </row>
-    <row r="1539" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1539" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1539" s="1">
         <v>1538</v>
       </c>
     </row>
-    <row r="1540" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1540" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1540" s="1">
         <v>1539</v>
       </c>
     </row>
-    <row r="1541" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1541" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1541" s="1">
         <v>1540</v>
       </c>
     </row>
-    <row r="1542" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1542" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1542" s="1">
         <v>1541</v>
       </c>
     </row>
-    <row r="1543" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1543" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1543" s="1">
         <v>1542</v>
       </c>
     </row>
-    <row r="1544" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1544" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1544" s="1">
         <v>1543</v>
       </c>
     </row>
-    <row r="1545" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1545" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1545" s="1">
         <v>1544</v>
       </c>
     </row>
-    <row r="1546" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1546" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1546" s="1">
         <v>1545</v>
       </c>
     </row>
-    <row r="1547" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1547" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1547" s="1">
         <v>1546</v>
       </c>
     </row>
-    <row r="1548" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1548" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1548" s="1">
         <v>1547</v>
       </c>
     </row>
-    <row r="1549" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1549" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1549" s="1">
         <v>1548</v>
       </c>
     </row>
-    <row r="1550" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1550" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1550" s="1">
         <v>1549</v>
       </c>
     </row>
-    <row r="1551" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1551" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1551" s="1">
         <v>1550</v>
       </c>
     </row>
-    <row r="1552" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1552" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1552" s="1">
         <v>1551</v>
       </c>

</xml_diff>